<commit_message>
Implementando conceito de multiplos endereco para uma pessoa.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -387,6 +387,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>41550</v>
+      </c>
+      <c r="B4">
+        <v>3.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Criação do mapeador e servicos do cadastro de inventor
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -395,6 +395,22 @@
         <v>3.5</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>41551</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>41552</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Implementando novo conceito de pais no modulo nucleo.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -411,6 +411,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>41553</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Adicionando controle de cliente para facilitar o demais cadastros dependentes do conceito de cliente.
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -419,6 +419,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>41554</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>41555</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>41556</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>41557</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Adicionando conceito de processo de marca
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -451,6 +451,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>41558</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>41559</v>
+      </c>
+      <c r="B13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28">
+        <f>SUM(B2:B27)</f>
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Implementação do conceito de processo de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Hermes.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -475,10 +475,34 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>41561</v>
+      </c>
+      <c r="B15">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>41562</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>41563</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="B28">
         <f>SUM(B2:B27)</f>
-        <v>45.5</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>